<commit_message>
v0.92 - Snowball+ 설계평가 기능 개선
</commit_message>
<xml_diff>
--- a/paper_templates/Design_Template.xlsx
+++ b/paper_templates/Design_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pythons\snowball\paper_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70AC0A0-948C-41C6-8BE8-25E7F26C915D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994734AA-7D2B-4FFE-8A5D-72C0082830D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="873" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
     <definedName name="NvsValTbl.ACCOUNT">"GL_ACCOUNT_TBL"</definedName>
     <definedName name="ORG">[3]SETUP!$A$3:$A$7</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">RCM!$A$1:$E$46</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Template!$A$1:$C$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Template!$A$1:$C$16</definedName>
     <definedName name="_xlnm.Print_Area">#REF!</definedName>
     <definedName name="Print_Area_MI">#REF!</definedName>
     <definedName name="Question_Type">[4]Values!$B$3:$B$10</definedName>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="119">
   <si>
     <t>Client</t>
     <phoneticPr fontId="19" type="noConversion"/>
@@ -576,6 +576,10 @@
   2. 샘플의 Monitoring 문서가 전체 권한을 대상으로 검토되었는지 확인한다
   3. Monitoring 문서의 승인 여부를 확인한다</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>첨부파일</t>
+    <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2734,10 +2738,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -2826,28 +2830,31 @@
       </c>
       <c r="C12" s="33"/>
     </row>
-    <row r="13" spans="1:4" ht="300" customHeight="1">
-      <c r="A13" s="9"/>
+    <row r="13" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
+      <c r="A13" s="15"/>
       <c r="B13" s="35" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="33"/>
     </row>
-    <row r="14" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A14" s="15"/>
+    <row r="14" spans="1:4" ht="300" customHeight="1">
+      <c r="A14" s="9"/>
       <c r="B14" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="33"/>
+    </row>
+    <row r="15" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1">
+      <c r="A15" s="15"/>
+      <c r="B15" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="36"/>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1">
-      <c r="A15" s="9"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="20"/>
+      <c r="C15" s="36"/>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1">
-      <c r="B16" s="13"/>
-      <c r="D16" s="19"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="20"/>
     </row>
     <row r="17" spans="2:4" ht="15" customHeight="1">
       <c r="B17" s="13"/>
@@ -2913,8 +2920,12 @@
       <c r="B32" s="13"/>
       <c r="D32" s="19"/>
     </row>
-    <row r="33" spans="4:4" ht="15" customHeight="1">
+    <row r="33" spans="2:4" ht="15" customHeight="1">
+      <c r="B33" s="13"/>
       <c r="D33" s="19"/>
+    </row>
+    <row r="34" spans="2:4" ht="15" customHeight="1">
+      <c r="D34" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
@@ -2926,21 +2937,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3076,19 +3087,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC26BC8C-8D44-46BE-A39D-C16F3FC5094C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF9F50EA-511A-47A0-93D9-E0B615D1BBD8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF9F50EA-511A-47A0-93D9-E0B615D1BBD8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC26BC8C-8D44-46BE-A39D-C16F3FC5094C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>